<commit_message>
Ready to test - 5/5
</commit_message>
<xml_diff>
--- a/data/ItemList-Excel.xlsx
+++ b/data/ItemList-Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yukina\Documents\GitHub\Critical-Story\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD5B276-5991-4AC5-B3EF-4187DBCED15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B07E735-7E0B-4E85-AA6A-F508F320D1A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -979,9 +979,6 @@
     <t>Heal &lt;green&gt;15% Health&lt;/font&gt; in every player phase</t>
   </si>
   <si>
-    <t>&lt;orange&gt;+50 Shield&lt;/font&gt;, restore &lt;orange&gt;10% Shield&lt;/font&gt; for every attack</t>
-  </si>
-  <si>
     <t>Used for &lt;orange&gt;Crafting&lt;/font&gt;</t>
   </si>
   <si>
@@ -1429,6 +1426,10 @@
   </si>
   <si>
     <t>Modus Shift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;orange&gt;+50 Shield&lt;/font&gt;, restore &lt;blue&gt;10% more TP&lt;/font&gt; for every attack</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1829,8 +1830,8 @@
   <dimension ref="A1:L86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -1983,7 +1984,7 @@
         <v>246</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H4" s="5" t="s">
         <v>116</v>
@@ -2132,7 +2133,7 @@
         <v>121</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>170</v>
@@ -2246,7 +2247,7 @@
         <v>124</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>173</v>
@@ -2284,7 +2285,7 @@
         <v>125</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>174</v>
@@ -2322,7 +2323,7 @@
         <v>126</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>175</v>
@@ -2337,7 +2338,7 @@
         <v>116</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L13" s="7">
         <v>0</v>
@@ -2360,7 +2361,7 @@
         <v>127</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>176</v>
@@ -2375,7 +2376,7 @@
         <v>116</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L14" s="7">
         <v>0</v>
@@ -2398,7 +2399,7 @@
         <v>128</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>177</v>
@@ -2550,7 +2551,7 @@
         <v>132</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>180</v>
@@ -2626,7 +2627,7 @@
         <v>134</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>182</v>
@@ -2664,10 +2665,10 @@
         <v>135</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H22" s="5" t="s">
         <v>115</v>
@@ -2778,7 +2779,7 @@
         <v>138</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>185</v>
@@ -2816,7 +2817,7 @@
         <v>139</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>186</v>
@@ -2854,7 +2855,7 @@
         <v>140</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>187</v>
@@ -2968,7 +2969,7 @@
         <v>143</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>190</v>
@@ -3006,7 +3007,7 @@
         <v>144</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>191</v>
@@ -3044,7 +3045,7 @@
         <v>145</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>192</v>
@@ -3082,7 +3083,7 @@
         <v>146</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>193</v>
@@ -3196,7 +3197,7 @@
         <v>149</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>196</v>
@@ -3272,7 +3273,7 @@
         <v>234</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>198</v>
@@ -3310,7 +3311,7 @@
         <v>151</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>199</v>
@@ -3348,7 +3349,7 @@
         <v>152</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>251</v>
+        <v>368</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>200</v>
@@ -3386,7 +3387,7 @@
         <v>153</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>201</v>
@@ -3424,7 +3425,7 @@
         <v>154</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>202</v>
@@ -3462,7 +3463,7 @@
         <v>155</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G43" s="5" t="s">
         <v>203</v>
@@ -3500,7 +3501,7 @@
         <v>156</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>204</v>
@@ -3538,7 +3539,7 @@
         <v>157</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>205</v>
@@ -3576,7 +3577,7 @@
         <v>158</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>206</v>
@@ -3614,7 +3615,7 @@
         <v>159</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>207</v>
@@ -3652,7 +3653,7 @@
         <v>160</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>208</v>
@@ -3690,7 +3691,7 @@
         <v>161</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G49" s="5" t="s">
         <v>209</v>
@@ -3728,7 +3729,7 @@
         <v>162</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>210</v>
@@ -3766,7 +3767,7 @@
         <v>163</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>211</v>
@@ -3804,7 +3805,7 @@
         <v>164</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>212</v>
@@ -3865,10 +3866,10 @@
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>279</v>
       </c>
       <c r="C54" s="5" t="s">
         <v>33</v>
@@ -3877,11 +3878,11 @@
         <v>34</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F54" s="5"/>
       <c r="G54" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H54" s="5" t="s">
         <v>115</v>
@@ -3901,10 +3902,10 @@
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>33</v>
@@ -3913,11 +3914,11 @@
         <v>34</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F55" s="5"/>
       <c r="G55" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>115</v>
@@ -3937,10 +3938,10 @@
     </row>
     <row r="56" spans="1:12" ht="31.2" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>284</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>33</v>
@@ -3949,11 +3950,11 @@
         <v>35</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F56" s="5"/>
       <c r="G56" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H56" s="5" t="s">
         <v>115</v>
@@ -3973,10 +3974,10 @@
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>287</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>288</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>33</v>
@@ -3987,7 +3988,7 @@
       <c r="E57" s="5"/>
       <c r="F57" s="5"/>
       <c r="G57" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>115</v>
@@ -4007,10 +4008,10 @@
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>33</v>
@@ -4021,7 +4022,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H58" s="5" t="s">
         <v>115</v>
@@ -4041,10 +4042,10 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>33</v>
@@ -4055,7 +4056,7 @@
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
       <c r="G59" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>115</v>
@@ -4075,10 +4076,10 @@
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C60" s="5" t="s">
         <v>33</v>
@@ -4089,7 +4090,7 @@
       <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H60" s="5" t="s">
         <v>115</v>
@@ -4109,10 +4110,10 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C61" s="5" t="s">
         <v>33</v>
@@ -4123,7 +4124,7 @@
       <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>115</v>
@@ -4143,10 +4144,10 @@
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>299</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>33</v>
@@ -4157,7 +4158,7 @@
       <c r="E62" s="5"/>
       <c r="F62" s="5"/>
       <c r="G62" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>115</v>
@@ -4177,10 +4178,10 @@
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>302</v>
-      </c>
-      <c r="B63" s="5" t="s">
-        <v>303</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>33</v>
@@ -4191,7 +4192,7 @@
       <c r="E63" s="5"/>
       <c r="F63" s="5"/>
       <c r="G63" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>115</v>
@@ -4211,10 +4212,10 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>304</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>305</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>33</v>
@@ -4225,7 +4226,7 @@
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
       <c r="G64" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>116</v>
@@ -4245,10 +4246,10 @@
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="B65" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>33</v>
@@ -4259,7 +4260,7 @@
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
       <c r="G65" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>115</v>
@@ -4279,10 +4280,10 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>310</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>311</v>
       </c>
       <c r="C66" s="5" t="s">
         <v>33</v>
@@ -4293,7 +4294,7 @@
       <c r="E66" s="5"/>
       <c r="F66" s="5"/>
       <c r="G66" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H66" s="5" t="s">
         <v>116</v>
@@ -4313,10 +4314,10 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>33</v>
@@ -4327,7 +4328,7 @@
       <c r="E67" s="5"/>
       <c r="F67" s="5"/>
       <c r="G67" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>115</v>
@@ -4347,10 +4348,10 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>33</v>
@@ -4361,7 +4362,7 @@
       <c r="E68" s="5"/>
       <c r="F68" s="5"/>
       <c r="G68" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H68" s="5" t="s">
         <v>115</v>
@@ -4381,10 +4382,10 @@
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>33</v>
@@ -4395,7 +4396,7 @@
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
       <c r="G69" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>115</v>
@@ -4415,10 +4416,10 @@
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="B70" s="5" t="s">
         <v>319</v>
-      </c>
-      <c r="B70" s="5" t="s">
-        <v>320</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>33</v>
@@ -4429,7 +4430,7 @@
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
       <c r="G70" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H70" s="5" t="s">
         <v>115</v>
@@ -4449,10 +4450,10 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>33</v>
@@ -4463,7 +4464,7 @@
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>115</v>
@@ -4483,10 +4484,10 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B72" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="B72" s="5" t="s">
-        <v>324</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>62</v>
@@ -4497,7 +4498,7 @@
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>115</v>
@@ -4517,10 +4518,10 @@
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="B73" s="5" t="s">
         <v>327</v>
-      </c>
-      <c r="B73" s="5" t="s">
-        <v>328</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>33</v>
@@ -4531,7 +4532,7 @@
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
       <c r="G73" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>115</v>
@@ -4551,10 +4552,10 @@
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="B74" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="B74" s="5" t="s">
-        <v>330</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>33</v>
@@ -4565,7 +4566,7 @@
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
       <c r="G74" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H74" s="5" t="s">
         <v>115</v>
@@ -4585,10 +4586,10 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="B75" s="5" t="s">
         <v>332</v>
-      </c>
-      <c r="B75" s="5" t="s">
-        <v>333</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>33</v>
@@ -4597,11 +4598,11 @@
         <v>34</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F75" s="5"/>
       <c r="G75" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>116</v>
@@ -4621,10 +4622,10 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="B76" s="5" t="s">
         <v>336</v>
-      </c>
-      <c r="B76" s="5" t="s">
-        <v>337</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>33</v>
@@ -4635,7 +4636,7 @@
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
       <c r="G76" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H76" s="5" t="s">
         <v>115</v>
@@ -4655,10 +4656,10 @@
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="B77" s="5" t="s">
         <v>339</v>
-      </c>
-      <c r="B77" s="5" t="s">
-        <v>340</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>33</v>
@@ -4669,7 +4670,7 @@
       <c r="E77" s="5"/>
       <c r="F77" s="5"/>
       <c r="G77" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>115</v>
@@ -4689,10 +4690,10 @@
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B78" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>342</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>33</v>
@@ -4703,7 +4704,7 @@
       <c r="E78" s="5"/>
       <c r="F78" s="5"/>
       <c r="G78" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H78" s="5" t="s">
         <v>115</v>
@@ -4723,10 +4724,10 @@
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>33</v>
@@ -4737,7 +4738,7 @@
       <c r="E79" s="5"/>
       <c r="F79" s="5"/>
       <c r="G79" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>115</v>
@@ -4757,10 +4758,10 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>33</v>
@@ -4771,7 +4772,7 @@
       <c r="E80" s="5"/>
       <c r="F80" s="5"/>
       <c r="G80" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H80" s="5" t="s">
         <v>115</v>
@@ -4791,10 +4792,10 @@
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="B81" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="B81" s="5" t="s">
-        <v>349</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>33</v>
@@ -4805,7 +4806,7 @@
       <c r="E81" s="5"/>
       <c r="F81" s="5"/>
       <c r="G81" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>115</v>
@@ -4825,10 +4826,10 @@
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="B82" s="5" t="s">
         <v>351</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>352</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>33</v>
@@ -4839,7 +4840,7 @@
       <c r="E82" s="5"/>
       <c r="F82" s="5"/>
       <c r="G82" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H82" s="5" t="s">
         <v>115</v>
@@ -4859,21 +4860,21 @@
     </row>
     <row r="83" spans="1:12" ht="31.2" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="B83" s="5" t="s">
         <v>354</v>
-      </c>
-      <c r="B83" s="5" t="s">
-        <v>355</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>62</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E83" s="5"/>
       <c r="F83" s="5"/>
       <c r="G83" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>115</v>
@@ -4893,10 +4894,10 @@
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>33</v>
@@ -4907,7 +4908,7 @@
       <c r="E84" s="5"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H84" s="5" t="s">
         <v>115</v>
@@ -4927,10 +4928,10 @@
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="B85" s="5" t="s">
         <v>359</v>
-      </c>
-      <c r="B85" s="5" t="s">
-        <v>360</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>33</v>
@@ -4941,7 +4942,7 @@
       <c r="E85" s="5"/>
       <c r="F85" s="5"/>
       <c r="G85" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>115</v>
@@ -4961,10 +4962,10 @@
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B86" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="B86" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>33</v>
@@ -4975,7 +4976,7 @@
       <c r="E86" s="5"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H86" s="5" t="s">
         <v>115</v>

</xml_diff>